<commit_message>
Add some deck related
</commit_message>
<xml_diff>
--- a/DataSource/excel/ship.xlsx
+++ b/DataSource/excel/ship.xlsx
@@ -44,7 +44,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1</t>
+shipstyle
+</t>
         </r>
         <r>
           <rPr>
@@ -54,8 +55,7 @@
             <family val="2"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">：中国造
-2：日本造
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>id</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>foodCapacity</t>
+  </si>
+  <si>
+    <t>卡鲁提拉号</t>
   </si>
 </sst>
 </file>
@@ -557,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -718,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -872,6 +875,56 @@
       </c>
       <c r="P6">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>25</v>
+      </c>
+      <c r="I7">
+        <v>50</v>
+      </c>
+      <c r="J7">
+        <v>1200</v>
+      </c>
+      <c r="K7">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <v>24</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>